<commit_message>
changed population file of issue #194
</commit_message>
<xml_diff>
--- a/Tests/ShouldSucceed/Issue194.xlsx
+++ b/Tests/ShouldSucceed/Issue194.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Auto</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Marie</t>
+  </si>
+  <si>
+    <t>[Auto]</t>
   </si>
 </sst>
 </file>
@@ -382,7 +385,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -390,51 +393,57 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This should fix the issue Han rased (I think it was #194)
</commit_message>
<xml_diff>
--- a/Tests/ShouldSucceed/Issue194.xlsx
+++ b/Tests/ShouldSucceed/Issue194.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Auto</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>[Auto]</t>
+  </si>
+  <si>
+    <t>Getal</t>
   </si>
 </sst>
 </file>
@@ -388,7 +391,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -437,6 +440,9 @@
       <c r="A7" t="s">
         <v>0</v>
       </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">

</xml_diff>